<commit_message>
Cleaned up some issues with storage operations and fixed excess supply switch values in list
</commit_message>
<xml_diff>
--- a/CaUWMET/output.xlsx
+++ b/CaUWMET/output.xlsx
@@ -6109,7 +6109,7 @@
         <v>1922</v>
       </c>
       <c r="C2" t="n">
-        <v>15467307.87667598</v>
+        <v>71306400.04671843</v>
       </c>
     </row>
     <row r="3">
@@ -6120,7 +6120,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>14275993.20384712</v>
+        <v>68587726.33105096</v>
       </c>
     </row>
     <row r="4">
@@ -6131,7 +6131,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>4925426.908090084</v>
+        <v>144706122.2570557</v>
       </c>
     </row>
     <row r="5">
@@ -6142,7 +6142,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>10169187.32794047</v>
+        <v>151562494.4921427</v>
       </c>
     </row>
     <row r="6">
@@ -6153,7 +6153,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>10401375.35706848</v>
+        <v>150036363.2332257</v>
       </c>
     </row>
     <row r="7">
@@ -6164,7 +6164,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>12776169.35510776</v>
+        <v>151564634.0191961</v>
       </c>
     </row>
     <row r="8">
@@ -6175,7 +6175,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>12122988.92202741</v>
+        <v>149625444.7663889</v>
       </c>
     </row>
     <row r="9">
@@ -6186,7 +6186,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>5154253.844520164</v>
+        <v>144835651.9603173</v>
       </c>
     </row>
     <row r="10">
@@ -6197,7 +6197,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>8874149.137438647</v>
+        <v>148555547.2532358</v>
       </c>
     </row>
     <row r="11">
@@ -6208,7 +6208,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>4479558.038707823</v>
+        <v>144160956.154505</v>
       </c>
     </row>
     <row r="12">
@@ -6219,7 +6219,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>6916712.443976915</v>
+        <v>145705177.1080653</v>
       </c>
     </row>
     <row r="13">
@@ -6230,7 +6230,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>7319740.964718893</v>
+        <v>144872008.8464804</v>
       </c>
     </row>
     <row r="14">
@@ -6241,7 +6241,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>5919481.344304165</v>
+        <v>145600879.4601014</v>
       </c>
     </row>
     <row r="15">
@@ -6252,7 +6252,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>9015118.476126088</v>
+        <v>147803583.1402144</v>
       </c>
     </row>
     <row r="16">
@@ -6263,7 +6263,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>12704688.58943342</v>
+        <v>151493153.2535218</v>
       </c>
     </row>
     <row r="17">
@@ -6274,7 +6274,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>10692897.47521078</v>
+        <v>149353794.7265991</v>
       </c>
     </row>
     <row r="18">
@@ -6285,7 +6285,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>15511385.36414507</v>
+        <v>68411547.69700919</v>
       </c>
     </row>
     <row r="19">
@@ -6296,7 +6296,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>11074952.05137929</v>
+        <v>148627219.9331408</v>
       </c>
     </row>
     <row r="20">
@@ -6307,7 +6307,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>11281455.07344669</v>
+        <v>150069919.737535</v>
       </c>
     </row>
     <row r="21">
@@ -6318,7 +6318,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>15411074.05044029</v>
+        <v>68467034.06192279</v>
       </c>
     </row>
     <row r="22">
@@ -6329,7 +6329,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>15859707.12275611</v>
+        <v>68218876.4270215</v>
       </c>
     </row>
     <row r="23">
@@ -6340,7 +6340,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>15851649.29996104</v>
+        <v>68223333.54436456</v>
       </c>
     </row>
     <row r="24">
@@ -6351,7 +6351,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>10388613.20262934</v>
+        <v>147891069.0469908</v>
       </c>
     </row>
     <row r="25">
@@ -6362,7 +6362,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>13024345.25761952</v>
+        <v>151812809.9217079</v>
       </c>
     </row>
     <row r="26">
@@ -6373,7 +6373,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>14338506.23734127</v>
+        <v>69127090.14792109</v>
       </c>
     </row>
     <row r="27">
@@ -6384,7 +6384,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>10591129.73026532</v>
+        <v>148143397.6120268</v>
       </c>
     </row>
     <row r="28">
@@ -6395,7 +6395,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>8419895.7036983</v>
+        <v>148049902.3761155</v>
       </c>
     </row>
     <row r="29">
@@ -6406,7 +6406,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>12082873.11313453</v>
+        <v>151712879.7855518</v>
       </c>
     </row>
     <row r="30">
@@ -6417,7 +6417,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>9444041.32861218</v>
+        <v>149074048.0010294</v>
       </c>
     </row>
     <row r="31">
@@ -6428,7 +6428,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>14460618.20025957</v>
+        <v>69039972.50266798</v>
       </c>
     </row>
     <row r="32">
@@ -6439,7 +6439,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>15803532.42320045</v>
+        <v>68249948.99265084</v>
       </c>
     </row>
     <row r="33">
@@ -6450,7 +6450,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>14880764.6525601</v>
+        <v>152383220.4969216</v>
       </c>
     </row>
     <row r="34">
@@ -6461,7 +6461,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>11852180.90385124</v>
+        <v>151482187.5762684</v>
       </c>
     </row>
     <row r="35">
@@ -6472,7 +6472,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>10894922.25415206</v>
+        <v>150529910.1303093</v>
       </c>
     </row>
     <row r="36">
@@ -6483,7 +6483,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>15432379.99024772</v>
+        <v>68455248.85936366</v>
       </c>
     </row>
     <row r="37">
@@ -6494,7 +6494,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>10517224.82642171</v>
+        <v>148019680.6707832</v>
       </c>
     </row>
     <row r="38">
@@ -6505,7 +6505,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>15361214.22994007</v>
+        <v>68494613.60497355</v>
       </c>
     </row>
     <row r="39">
@@ -6516,7 +6516,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>13413218.20091805</v>
+        <v>150965486.0826795</v>
       </c>
     </row>
     <row r="40">
@@ -6527,7 +6527,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>8324440.267083074</v>
+        <v>148005838.3828803</v>
       </c>
     </row>
     <row r="41">
@@ -6538,7 +6538,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>10078116.91979573</v>
+        <v>149759515.0355929</v>
       </c>
     </row>
     <row r="42">
@@ -6549,7 +6549,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>9517930.171392344</v>
+        <v>149147936.8438095</v>
       </c>
     </row>
     <row r="43">
@@ -6560,7 +6560,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>14924616.02763454</v>
+        <v>68708945.1638436</v>
       </c>
     </row>
     <row r="44">
@@ -6571,7 +6571,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>10237173.41950819</v>
+        <v>147789441.3012697</v>
       </c>
     </row>
     <row r="45">
@@ -6582,7 +6582,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>14952554.26341131</v>
+        <v>68720660.45044824</v>
       </c>
     </row>
     <row r="46">
@@ -6593,7 +6593,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>12326925.9464633</v>
+        <v>149829381.7908248</v>
       </c>
     </row>
     <row r="47">
@@ -6604,7 +6604,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>15553170.65611573</v>
+        <v>68388434.51193888</v>
       </c>
     </row>
     <row r="48">
@@ -6615,7 +6615,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>14337093.79494978</v>
+        <v>151889361.6767113</v>
       </c>
     </row>
     <row r="49">
@@ -6626,7 +6626,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>15757059.20288194</v>
+        <v>68275655.26611161</v>
       </c>
     </row>
     <row r="50">
@@ -6637,7 +6637,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>15592253.09714176</v>
+        <v>68232636.63526751</v>
       </c>
     </row>
     <row r="51">
@@ -6648,7 +6648,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>11759233.15795435</v>
+        <v>149261689.0023158</v>
       </c>
     </row>
     <row r="52">
@@ -6659,7 +6659,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>11418255.28478753</v>
+        <v>151053243.1609447</v>
       </c>
     </row>
     <row r="53">
@@ -6670,7 +6670,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>14426104.8532215</v>
+        <v>69064595.16413295</v>
       </c>
     </row>
     <row r="54">
@@ -6681,7 +6681,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>15787532.34086164</v>
+        <v>68258799.30449015</v>
       </c>
     </row>
     <row r="55">
@@ -6692,7 +6692,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>14530503.88266835</v>
+        <v>68954114.09164709</v>
       </c>
     </row>
     <row r="56">
@@ -6703,7 +6703,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>9042602.139237579</v>
+        <v>147058972.4173991</v>
       </c>
     </row>
     <row r="57">
@@ -6714,7 +6714,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>3714623.03651678</v>
+        <v>143396021.152314</v>
       </c>
     </row>
     <row r="58">
@@ -6725,7 +6725,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>14713881.7908291</v>
+        <v>68852680.13416508</v>
       </c>
     </row>
     <row r="59">
@@ -6736,7 +6736,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>14173075.61250979</v>
+        <v>69245112.38049883</v>
       </c>
     </row>
     <row r="60">
@@ -6747,7 +6747,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>15734927.34397805</v>
+        <v>68287897.31891704</v>
       </c>
     </row>
     <row r="61">
@@ -6758,7 +6758,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>12330278.57805294</v>
+        <v>149882546.4598144</v>
       </c>
     </row>
     <row r="62">
@@ -6769,7 +6769,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>15556360.77489346</v>
+        <v>68386669.92439556</v>
       </c>
     </row>
     <row r="63">
@@ -6780,7 +6780,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>15911556.98701414</v>
+        <v>68190196.10789612</v>
       </c>
     </row>
     <row r="64">
@@ -6791,7 +6791,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>15196622.95883098</v>
+        <v>68514888.80137065</v>
       </c>
     </row>
     <row r="65">
@@ -6802,7 +6802,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>12036152.86442794</v>
+        <v>149588420.7461894</v>
       </c>
     </row>
     <row r="66">
@@ -6813,7 +6813,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>15343962.69787148</v>
+        <v>68504156.14577302</v>
       </c>
     </row>
     <row r="67">
@@ -6824,7 +6824,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>10681476.41161022</v>
+        <v>148697846.6897717</v>
       </c>
     </row>
     <row r="68">
@@ -6835,7 +6835,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>8202072.489149316</v>
+        <v>147883470.6049465</v>
       </c>
     </row>
     <row r="69">
@@ -6846,7 +6846,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>8265318.290755522</v>
+        <v>147946716.4065527</v>
       </c>
     </row>
     <row r="70">
@@ -6857,7 +6857,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>7262318.24174059</v>
+        <v>146943716.3575378</v>
       </c>
     </row>
     <row r="71">
@@ -6868,7 +6868,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>4358466.775472678</v>
+        <v>144039864.8912699</v>
       </c>
     </row>
     <row r="72">
@@ -6879,7 +6879,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>6598960.621098698</v>
+        <v>146280358.7368959</v>
       </c>
     </row>
     <row r="73">
@@ -6890,7 +6890,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>13497860.72156341</v>
+        <v>152158757.9729517</v>
       </c>
     </row>
     <row r="74">
@@ -6901,7 +6901,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>11207527.10470622</v>
+        <v>149223897.3828677</v>
       </c>
     </row>
     <row r="75">
@@ -6912,7 +6912,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>15440612.55072757</v>
+        <v>68450695.08733051</v>
       </c>
     </row>
     <row r="76">
@@ -6923,7 +6923,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>15620210.06021401</v>
+        <v>68351352.22578388</v>
       </c>
     </row>
     <row r="77">
@@ -6934,7 +6934,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>15893586.88551395</v>
+        <v>68200136.11937186</v>
       </c>
     </row>
     <row r="78">
@@ -6945,7 +6945,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>15911556.98701414</v>
+        <v>68190196.10789612</v>
       </c>
     </row>
     <row r="79">
@@ -6956,7 +6956,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>15319467.61027232</v>
+        <v>68427248.43829936</v>
       </c>
     </row>
     <row r="80">
@@ -6967,7 +6967,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>14243718.05116007</v>
+        <v>69194714.34607965</v>
       </c>
     </row>
     <row r="81">
@@ -6978,7 +6978,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>11275000.89769531</v>
+        <v>148827268.7794568</v>
       </c>
     </row>
     <row r="82">
@@ -6989,7 +6989,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>11124494.19232186</v>
+        <v>150759482.068479</v>
       </c>
     </row>
     <row r="83">
@@ -7000,7 +7000,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>12152981.52540478</v>
+        <v>151782988.197822</v>
       </c>
     </row>
     <row r="84">
@@ -7011,7 +7011,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>12581292.31448059</v>
+        <v>68599802.95749058</v>
       </c>
     </row>
     <row r="85">
@@ -7022,7 +7022,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>15122915.3402404</v>
+        <v>68626426.64444079</v>
       </c>
     </row>
     <row r="86">
@@ -7033,7 +7033,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>15876296.16381384</v>
+        <v>68209700.33758852</v>
       </c>
     </row>
     <row r="87">
@@ -7044,7 +7044,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>14176555.26816908</v>
+        <v>152192925.5463306</v>
       </c>
     </row>
     <row r="88">
@@ -7055,7 +7055,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>9261435.489619618</v>
+        <v>148942833.6054168</v>
       </c>
     </row>
     <row r="89">
@@ -7066,7 +7066,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>7442771.263907343</v>
+        <v>147072777.9363245</v>
       </c>
     </row>
     <row r="90">
@@ -7077,7 +7077,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>10565127.57689347</v>
+        <v>149353592.2409818</v>
       </c>
     </row>
     <row r="91">
@@ -7088,7 +7088,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>15455227.81602237</v>
+        <v>68442610.77546673</v>
       </c>
     </row>
     <row r="92">
@@ -7099,7 +7099,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>13984897.69078986</v>
+        <v>151537165.5725513</v>
       </c>
     </row>
     <row r="93">
@@ -7110,7 +7110,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>11186207.21294427</v>
+        <v>150867605.3287415</v>
       </c>
     </row>
     <row r="94">
@@ -7121,7 +7121,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>4617907.41124785</v>
+        <v>144299305.527045</v>
       </c>
     </row>
   </sheetData>
@@ -7179,7 +7179,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>-1120.0130309</v>
       </c>
     </row>
     <row r="4">
@@ -7190,7 +7190,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5">
@@ -7201,7 +7201,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6">
@@ -7212,7 +7212,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
@@ -7223,7 +7223,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8">
@@ -7234,7 +7234,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9">
@@ -7245,7 +7245,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10">
@@ -7256,7 +7256,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
@@ -7267,7 +7267,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12">
@@ -7278,7 +7278,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="13">
@@ -7289,7 +7289,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="14">
@@ -7300,7 +7300,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15">
@@ -7311,7 +7311,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="16">
@@ -7322,7 +7322,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17">
@@ -7333,7 +7333,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="18">
@@ -7344,7 +7344,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>-950.2274209000011</v>
       </c>
     </row>
     <row r="19">
@@ -7355,7 +7355,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="20">
@@ -7366,7 +7366,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="21">
@@ -7377,7 +7377,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>-824.1907908999988</v>
       </c>
     </row>
     <row r="22">
@@ -7388,7 +7388,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>-1387.8779609</v>
       </c>
     </row>
     <row r="23">
@@ -7399,7 +7399,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>-1377.7536709</v>
       </c>
     </row>
     <row r="24">
@@ -7410,7 +7410,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="25">
@@ -7421,7 +7421,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="26">
@@ -7432,7 +7432,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>523.4421691000002</v>
       </c>
     </row>
     <row r="27">
@@ -7443,7 +7443,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="28">
@@ -7454,7 +7454,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29">
@@ -7465,7 +7465,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30">
@@ -7476,7 +7476,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31">
@@ -7487,7 +7487,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>370.0140091000007</v>
       </c>
     </row>
     <row r="32">
@@ -7498,7 +7498,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>-1317.296990900001</v>
       </c>
     </row>
     <row r="33">
@@ -7509,7 +7509,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="34">
@@ -7520,7 +7520,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35">
@@ -7531,7 +7531,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36">
@@ -7542,7 +7542,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>-850.9607409000005</v>
       </c>
     </row>
     <row r="37">
@@ -7553,7 +7553,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="38">
@@ -7564,7 +7564,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>-761.544180899999</v>
       </c>
     </row>
     <row r="39">
@@ -7575,7 +7575,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="40">
@@ -7586,7 +7586,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41">
@@ -7597,7 +7597,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42">
@@ -7608,7 +7608,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43">
@@ -7619,7 +7619,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>-212.9782809000012</v>
       </c>
     </row>
     <row r="44">
@@ -7630,7 +7630,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="45">
@@ -7641,7 +7641,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>-248.0814109000007</v>
       </c>
     </row>
     <row r="46">
@@ -7652,7 +7652,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="47">
@@ -7663,7 +7663,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>-1002.7287509</v>
       </c>
     </row>
     <row r="48">
@@ -7674,7 +7674,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="49">
@@ -7685,7 +7685,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>-1258.905490899999</v>
       </c>
     </row>
     <row r="50">
@@ -7696,7 +7696,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>-1051.834070899999</v>
       </c>
     </row>
     <row r="51">
@@ -7707,7 +7707,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="52">
@@ -7718,7 +7718,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53">
@@ -7729,7 +7729,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>413.3784691000014</v>
       </c>
     </row>
     <row r="54">
@@ -7740,7 +7740,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>-1297.1936109</v>
       </c>
     </row>
     <row r="55">
@@ -7751,7 +7751,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>282.2058091000013</v>
       </c>
     </row>
     <row r="56">
@@ -7762,7 +7762,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="57">
@@ -7773,7 +7773,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58">
@@ -7784,7 +7784,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>51.79975909999985</v>
       </c>
     </row>
     <row r="59">
@@ -7795,7 +7795,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>731.2982691000011</v>
       </c>
     </row>
     <row r="60">
@@ -7806,7 +7806,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>-1231.097810900001</v>
       </c>
     </row>
     <row r="61">
@@ -7817,7 +7817,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="62">
@@ -7828,7 +7828,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>-1006.736990899999</v>
       </c>
     </row>
     <row r="63">
@@ -7839,7 +7839,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>-1453.0249709</v>
       </c>
     </row>
     <row r="64">
@@ -7850,7 +7850,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>-554.742690900001</v>
       </c>
     </row>
     <row r="65">
@@ -7861,7 +7861,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="66">
@@ -7872,7 +7872,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>-739.868410900001</v>
       </c>
     </row>
     <row r="67">
@@ -7883,7 +7883,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="68">
@@ -7894,7 +7894,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69">
@@ -7905,7 +7905,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70">
@@ -7916,7 +7916,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71">
@@ -7927,7 +7927,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72">
@@ -7938,7 +7938,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73">
@@ -7949,7 +7949,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="74">
@@ -7960,7 +7960,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="75">
@@ -7971,7 +7971,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>-861.3045808999982</v>
       </c>
     </row>
     <row r="76">
@@ -7982,7 +7982,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>-1086.960730900001</v>
       </c>
     </row>
     <row r="77">
@@ -7993,7 +7993,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>-1430.4463509</v>
       </c>
     </row>
     <row r="78">
@@ -8004,7 +8004,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>-1453.0249709</v>
       </c>
     </row>
     <row r="79">
@@ -8015,7 +8015,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>-709.0914408999984</v>
       </c>
     </row>
     <row r="80">
@@ -8026,7 +8026,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>642.5392391</v>
       </c>
     </row>
     <row r="81">
@@ -8037,7 +8037,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="82">
@@ -8048,7 +8048,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83">
@@ -8059,7 +8059,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84">
@@ -8070,7 +8070,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>-71.69799089999879</v>
       </c>
     </row>
     <row r="85">
@@ -8081,7 +8081,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>-462.1324009000004</v>
       </c>
     </row>
     <row r="86">
@@ -8092,7 +8092,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>-1408.721340899998</v>
       </c>
     </row>
     <row r="87">
@@ -8103,7 +8103,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="88">
@@ -8114,7 +8114,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="89">
@@ -8125,7 +8125,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90">
@@ -8136,7 +8136,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="91">
@@ -8147,7 +8147,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>-879.6680008999997</v>
       </c>
     </row>
     <row r="92">
@@ -8158,7 +8158,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="93">
@@ -8169,7 +8169,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="94">
@@ -8180,7 +8180,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -8238,7 +8238,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>-706221.4131293775</v>
       </c>
     </row>
     <row r="4">
@@ -8249,7 +8249,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1282963.693</v>
       </c>
     </row>
     <row r="5">
@@ -8260,7 +8260,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>76904.92592000001</v>
       </c>
     </row>
     <row r="6">
@@ -8271,7 +8271,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>81886.12965999999</v>
       </c>
     </row>
     <row r="7">
@@ -8282,7 +8282,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>630547.4969</v>
       </c>
     </row>
     <row r="8">
@@ -8293,7 +8293,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>769049.2592000001</v>
       </c>
     </row>
     <row r="9">
@@ -8304,7 +8304,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="10">
@@ -8315,7 +8315,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="11">
@@ -8326,7 +8326,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="12">
@@ -8337,7 +8337,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>630547.4969</v>
       </c>
     </row>
     <row r="13">
@@ -8348,7 +8348,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>818861.2966</v>
       </c>
     </row>
     <row r="14">
@@ -8359,7 +8359,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="15">
@@ -8370,7 +8370,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>630547.4969</v>
       </c>
     </row>
     <row r="16">
@@ -8381,7 +8381,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>630547.4969</v>
       </c>
     </row>
     <row r="17">
@@ -8392,7 +8392,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>502980.0842</v>
       </c>
     </row>
     <row r="18">
@@ -8403,7 +8403,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>-477945.4681734314</v>
       </c>
     </row>
     <row r="19">
@@ -8414,7 +8414,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>818861.2966</v>
       </c>
     </row>
     <row r="20">
@@ -8425,7 +8425,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>630547.4969</v>
       </c>
     </row>
     <row r="21">
@@ -8436,7 +8436,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>-414551.553403746</v>
       </c>
     </row>
     <row r="22">
@@ -8447,7 +8447,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>-698074.9736328062</v>
       </c>
     </row>
     <row r="23">
@@ -8458,7 +8458,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>-692982.6573961412</v>
       </c>
     </row>
     <row r="24">
@@ -8469,7 +8469,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>769049.2592000001</v>
       </c>
     </row>
     <row r="25">
@@ -8480,7 +8480,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>630547.4969</v>
       </c>
     </row>
     <row r="26">
@@ -8491,7 +8491,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>330055.1494979117</v>
       </c>
     </row>
     <row r="27">
@@ -8502,7 +8502,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>818861.2966</v>
       </c>
     </row>
     <row r="28">
@@ -8513,7 +8513,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>76904.92592000001</v>
       </c>
     </row>
     <row r="29">
@@ -8524,7 +8524,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>76904.92592000001</v>
       </c>
     </row>
     <row r="30">
@@ -8535,7 +8535,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>76904.92592000001</v>
       </c>
     </row>
     <row r="31">
@@ -8546,7 +8546,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>233311.4072559393</v>
       </c>
     </row>
     <row r="32">
@@ -8557,7 +8557,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>-662574.151399289</v>
       </c>
     </row>
     <row r="33">
@@ -8568,7 +8568,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>769049.2592000001</v>
       </c>
     </row>
     <row r="34">
@@ -8579,7 +8579,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>76904.92592000001</v>
       </c>
     </row>
     <row r="35">
@@ -8590,7 +8590,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>81886.12965999999</v>
       </c>
     </row>
     <row r="36">
@@ -8601,7 +8601,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>-428016.3051087767</v>
       </c>
     </row>
     <row r="37">
@@ -8612,7 +8612,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>769049.2592000001</v>
       </c>
     </row>
     <row r="38">
@@ -8623,7 +8623,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>-383041.5562311016</v>
       </c>
     </row>
     <row r="39">
@@ -8634,7 +8634,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>818861.2966</v>
       </c>
     </row>
     <row r="40">
@@ -8645,7 +8645,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="41">
@@ -8656,7 +8656,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="42">
@@ -8667,7 +8667,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>76904.92592000001</v>
       </c>
     </row>
     <row r="43">
@@ -8678,7 +8678,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>-134292.9219155608</v>
       </c>
     </row>
     <row r="44">
@@ -8689,7 +8689,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>818861.2966</v>
       </c>
     </row>
     <row r="45">
@@ -8700,7 +8700,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>-124780.0089429372</v>
       </c>
     </row>
     <row r="46">
@@ -8711,7 +8711,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>769049.2592000001</v>
       </c>
     </row>
     <row r="47">
@@ -8722,7 +8722,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>-504352.591557443</v>
       </c>
     </row>
     <row r="48">
@@ -8733,7 +8733,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>818861.2966</v>
       </c>
     </row>
     <row r="49">
@@ -8744,7 +8744,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>-633204.389812724</v>
       </c>
     </row>
     <row r="50">
@@ -8755,7 +8755,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>-663231.3405601316</v>
       </c>
     </row>
     <row r="51">
@@ -8766,7 +8766,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>769049.2592000001</v>
       </c>
     </row>
     <row r="52">
@@ -8777,7 +8777,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>81886.12965999999</v>
       </c>
     </row>
     <row r="53">
@@ -8788,7 +8788,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>260654.7589633599</v>
       </c>
     </row>
     <row r="54">
@@ -8799,7 +8799,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>-652462.5516341842</v>
       </c>
     </row>
     <row r="55">
@@ -8810,7 +8810,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>141943.9016228478</v>
       </c>
     </row>
     <row r="56">
@@ -8821,7 +8821,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>1282963.693</v>
       </c>
     </row>
     <row r="57">
@@ -8832,7 +8832,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="58">
@@ -8843,7 +8843,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>26054.24719365764</v>
       </c>
     </row>
     <row r="59">
@@ -8854,7 +8854,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>461118.2930683084</v>
       </c>
     </row>
     <row r="60">
@@ -8865,7 +8865,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>-619217.6805849182</v>
       </c>
     </row>
     <row r="61">
@@ -8876,7 +8876,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>818861.2966</v>
       </c>
     </row>
     <row r="62">
@@ -8887,7 +8887,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>-506368.6564501364</v>
       </c>
     </row>
     <row r="63">
@@ -8898,7 +8898,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>-730842.6222079848</v>
       </c>
     </row>
     <row r="64">
@@ -8909,7 +8909,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>-349791.6151705661</v>
       </c>
     </row>
     <row r="65">
@@ -8920,7 +8920,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>818861.2966</v>
       </c>
     </row>
     <row r="66">
@@ -8931,7 +8931,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>-372139.0756114027</v>
       </c>
     </row>
     <row r="67">
@@ -8942,7 +8942,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>1282963.693</v>
       </c>
     </row>
     <row r="68">
@@ -8953,7 +8953,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="69">
@@ -8964,7 +8964,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="70">
@@ -8975,7 +8975,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="71">
@@ -8986,7 +8986,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="72">
@@ -8997,7 +8997,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="73">
@@ -9008,7 +9008,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>502980.0842</v>
       </c>
     </row>
     <row r="74">
@@ -9019,7 +9019,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>1282963.693</v>
       </c>
     </row>
     <row r="75">
@@ -9030,7 +9030,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>-433219.0506229269</v>
       </c>
     </row>
     <row r="76">
@@ -9041,7 +9041,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>-546719.599950176</v>
       </c>
     </row>
     <row r="77">
@@ -9052,7 +9052,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>-719486.0260192648</v>
       </c>
     </row>
     <row r="78">
@@ -9063,7 +9063,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>-730842.6222079848</v>
       </c>
     </row>
     <row r="79">
@@ -9074,7 +9074,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>-447115.8331327083</v>
       </c>
     </row>
     <row r="80">
@@ -9085,7 +9085,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>405151.5088745357</v>
       </c>
     </row>
     <row r="81">
@@ -9096,7 +9096,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>818861.2966</v>
       </c>
     </row>
     <row r="82">
@@ -9107,7 +9107,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>81886.12965999999</v>
       </c>
     </row>
     <row r="83">
@@ -9118,7 +9118,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>76904.92592000001</v>
       </c>
     </row>
     <row r="84">
@@ -9129,7 +9129,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>-58710.709791988</v>
       </c>
     </row>
     <row r="85">
@@ -9140,7 +9140,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>-232443.3939162304</v>
       </c>
     </row>
     <row r="86">
@@ -9151,7 +9151,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>-708558.7786602181</v>
       </c>
     </row>
     <row r="87">
@@ -9162,7 +9162,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>1282963.693</v>
       </c>
     </row>
     <row r="88">
@@ -9173,7 +9173,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="89">
@@ -9184,7 +9184,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>76904.92592000001</v>
       </c>
     </row>
     <row r="90">
@@ -9195,7 +9195,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>630547.4969</v>
       </c>
     </row>
     <row r="91">
@@ -9206,7 +9206,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>-442455.4851607275</v>
       </c>
     </row>
     <row r="92">
@@ -9217,7 +9217,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>818861.2966</v>
       </c>
     </row>
     <row r="93">
@@ -9228,7 +9228,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
     <row r="94">
@@ -9239,7 +9239,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>128296.3693</v>
       </c>
     </row>
   </sheetData>
@@ -22560,7 +22560,7 @@
         <v>1922</v>
       </c>
       <c r="C2" t="n">
-        <v>15467307.87667598</v>
+        <v>71306400.04671843</v>
       </c>
     </row>
     <row r="3">
@@ -22571,7 +22571,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>14275993.20384712</v>
+        <v>68587726.33105096</v>
       </c>
     </row>
     <row r="4">
@@ -22582,7 +22582,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>4925426.908090084</v>
+        <v>275764616.5824751</v>
       </c>
     </row>
     <row r="5">
@@ -22593,7 +22593,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>10169187.32794047</v>
+        <v>153975840.0426206</v>
       </c>
     </row>
     <row r="6">
@@ -22604,7 +22604,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>10401375.35706848</v>
+        <v>156426279.8716294</v>
       </c>
     </row>
     <row r="7">
@@ -22615,7 +22615,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>12776169.35510776</v>
+        <v>154837841.1567045</v>
       </c>
     </row>
     <row r="8">
@@ -22626,7 +22626,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>12122988.92202741</v>
+        <v>162678416.4133644</v>
       </c>
     </row>
     <row r="9">
@@ -22637,7 +22637,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>5154253.844520164</v>
+        <v>207505091.4632434</v>
       </c>
     </row>
     <row r="10">
@@ -22648,7 +22648,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>8874149.137438647</v>
+        <v>162774524.212621</v>
       </c>
     </row>
     <row r="11">
@@ -22659,7 +22659,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>4479558.038707823</v>
+        <v>226074713.3663148</v>
       </c>
     </row>
     <row r="12">
@@ -22670,7 +22670,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>6916712.443976915</v>
+        <v>202606069.1851418</v>
       </c>
     </row>
     <row r="13">
@@ -22681,7 +22681,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>7319740.964718893</v>
+        <v>234484955.8242993</v>
       </c>
     </row>
     <row r="14">
@@ -22692,7 +22692,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>5919481.344304165</v>
+        <v>192202375.2897353</v>
       </c>
     </row>
     <row r="15">
@@ -22703,7 +22703,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>9015118.476126088</v>
+        <v>173066864.015955</v>
       </c>
     </row>
     <row r="16">
@@ -22714,7 +22714,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>12704688.58943342</v>
+        <v>154998464.9308866</v>
       </c>
     </row>
     <row r="17">
@@ -22725,7 +22725,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>10692897.47521078</v>
+        <v>161716380.5158835</v>
       </c>
     </row>
     <row r="18">
@@ -22736,7 +22736,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>15511385.36414507</v>
+        <v>68411547.69700919</v>
       </c>
     </row>
     <row r="19">
@@ -22747,7 +22747,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>11074952.05137929</v>
+        <v>169171899.7272645</v>
       </c>
     </row>
     <row r="20">
@@ -22758,7 +22758,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>11281455.07344669</v>
+        <v>159291435.9376023</v>
       </c>
     </row>
     <row r="21">
@@ -22769,7 +22769,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>15411074.05044029</v>
+        <v>68467034.06192279</v>
       </c>
     </row>
     <row r="22">
@@ -22780,7 +22780,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>15859707.12275611</v>
+        <v>68218876.4270215</v>
       </c>
     </row>
     <row r="23">
@@ -22791,7 +22791,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>15851649.29996104</v>
+        <v>68223333.54436456</v>
       </c>
     </row>
     <row r="24">
@@ -22802,7 +22802,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>10388613.20262934</v>
+        <v>174940788.7406322</v>
       </c>
     </row>
     <row r="25">
@@ -22813,7 +22813,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>13024345.25761952</v>
+        <v>154313595.5113933</v>
       </c>
     </row>
     <row r="26">
@@ -22824,7 +22824,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>14338506.23734127</v>
+        <v>69127090.14792109</v>
       </c>
     </row>
     <row r="27">
@@ -22835,7 +22835,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>10591129.73026532</v>
+        <v>173113073.0613106</v>
       </c>
     </row>
     <row r="28">
@@ -22846,7 +22846,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>8419895.7036983</v>
+        <v>165391049.3419265</v>
       </c>
     </row>
     <row r="29">
@@ -22857,7 +22857,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>12082873.11313453</v>
+        <v>152610395.9289285</v>
       </c>
     </row>
     <row r="30">
@@ -22868,7 +22868,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>9444041.32861218</v>
+        <v>159949941.5318053</v>
       </c>
     </row>
     <row r="31">
@@ -22879,7 +22879,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>14460618.20025957</v>
+        <v>69039972.50266798</v>
       </c>
     </row>
     <row r="32">
@@ -22890,7 +22890,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>15803532.42320045</v>
+        <v>68249948.99265084</v>
       </c>
     </row>
     <row r="33">
@@ -22901,7 +22901,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>14880764.6525601</v>
+        <v>153987734.4805636</v>
       </c>
     </row>
     <row r="34">
@@ -22912,7 +22912,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>11852180.90385124</v>
+        <v>152996642.6919705</v>
       </c>
     </row>
     <row r="35">
@@ -22923,7 +22923,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>10894922.25415206</v>
+        <v>155042496.3080782</v>
       </c>
     </row>
     <row r="36">
@@ -22934,7 +22934,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>15432379.99024772</v>
+        <v>68455248.85936366</v>
       </c>
     </row>
     <row r="37">
@@ -22945,7 +22945,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>10517224.82642171</v>
+        <v>173731614.996713</v>
       </c>
     </row>
     <row r="38">
@@ -22956,7 +22956,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>15361214.22994007</v>
+        <v>68494613.60497355</v>
       </c>
     </row>
     <row r="39">
@@ -22967,7 +22967,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>13413218.20091805</v>
+        <v>157557506.1788989</v>
       </c>
     </row>
     <row r="40">
@@ -22978,7 +22978,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>8324440.267083074</v>
+        <v>166062473.193146</v>
       </c>
     </row>
     <row r="41">
@@ -22989,7 +22989,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>10078116.91979573</v>
+        <v>157527603.9264222</v>
       </c>
     </row>
     <row r="42">
@@ -23000,7 +23000,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>9517930.171392344</v>
+        <v>159631087.841297</v>
       </c>
     </row>
     <row r="43">
@@ -23011,7 +23011,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>14924616.02763454</v>
+        <v>68708945.1638436</v>
       </c>
     </row>
     <row r="44">
@@ -23022,7 +23022,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>10237173.41950819</v>
+        <v>176493323.9217184</v>
       </c>
     </row>
     <row r="45">
@@ -23033,7 +23033,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>14952554.26341131</v>
+        <v>68720660.45044824</v>
       </c>
     </row>
     <row r="46">
@@ -23044,7 +23044,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>12326925.9464633</v>
+        <v>161689351.2049618</v>
       </c>
     </row>
     <row r="47">
@@ -23055,7 +23055,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>15553170.65611573</v>
+        <v>68388434.51193888</v>
       </c>
     </row>
     <row r="48">
@@ -23066,7 +23066,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>14337093.79494978</v>
+        <v>155116472.6800007</v>
       </c>
     </row>
     <row r="49">
@@ -23077,7 +23077,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>15757059.20288194</v>
+        <v>68275655.26611161</v>
       </c>
     </row>
     <row r="50">
@@ -23088,7 +23088,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>15592253.09714176</v>
+        <v>68232636.63526751</v>
       </c>
     </row>
     <row r="51">
@@ -23099,7 +23099,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>11759233.15795435</v>
+        <v>164637900.6008855</v>
       </c>
     </row>
     <row r="52">
@@ -23110,7 +23110,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>11418255.28478753</v>
+        <v>153832954.0035108</v>
       </c>
     </row>
     <row r="53">
@@ -23121,7 +23121,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>14426104.8532215</v>
+        <v>69064595.16413295</v>
       </c>
     </row>
     <row r="54">
@@ -23132,7 +23132,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>15787532.34086164</v>
+        <v>68258799.30449015</v>
       </c>
     </row>
     <row r="55">
@@ -23143,7 +23143,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>14530503.88266835</v>
+        <v>68954114.09164709</v>
       </c>
     </row>
     <row r="56">
@@ -23154,7 +23154,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>9042602.139237579</v>
+        <v>192563301.9722689</v>
       </c>
     </row>
     <row r="57">
@@ -23165,7 +23165,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>3714623.03651678</v>
+        <v>252962214.7984976</v>
       </c>
     </row>
     <row r="58">
@@ -23176,7 +23176,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>14713881.7908291</v>
+        <v>68852680.13416508</v>
       </c>
     </row>
     <row r="59">
@@ -23187,7 +23187,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>14173075.61250979</v>
+        <v>69245112.38049883</v>
       </c>
     </row>
     <row r="60">
@@ -23198,7 +23198,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>15734927.34397805</v>
+        <v>68287897.31891704</v>
       </c>
     </row>
     <row r="61">
@@ -23209,7 +23209,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>12330278.57805294</v>
+        <v>161723515.0288115</v>
       </c>
     </row>
     <row r="62">
@@ -23220,7 +23220,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>15556360.77489346</v>
+        <v>68386669.92439556</v>
       </c>
     </row>
     <row r="63">
@@ -23231,7 +23231,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>15911556.98701414</v>
+        <v>68190196.10789612</v>
       </c>
     </row>
     <row r="64">
@@ -23242,7 +23242,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>15196622.95883098</v>
+        <v>68514888.80137065</v>
       </c>
     </row>
     <row r="65">
@@ -23253,7 +23253,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>12036152.86442794</v>
+        <v>163172420.2849106</v>
       </c>
     </row>
     <row r="66">
@@ -23264,7 +23264,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>15343962.69787148</v>
+        <v>68504156.14577302</v>
       </c>
     </row>
     <row r="67">
@@ -23275,7 +23275,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>10681476.41161022</v>
+        <v>172785323.8675387</v>
       </c>
     </row>
     <row r="68">
@@ -23286,7 +23286,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>8202072.489149316</v>
+        <v>166890229.5324392</v>
       </c>
     </row>
     <row r="69">
@@ -23297,7 +23297,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>8265318.290755522</v>
+        <v>166457691.4296048</v>
       </c>
     </row>
     <row r="70">
@@ -23308,7 +23308,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>7262318.24174059</v>
+        <v>174694467.1112428</v>
       </c>
     </row>
     <row r="71">
@@ -23319,7 +23319,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>4358466.775472678</v>
+        <v>230074211.3262015</v>
       </c>
     </row>
     <row r="72">
@@ -23330,7 +23330,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>6598960.621098698</v>
+        <v>182175639.3835852</v>
       </c>
     </row>
     <row r="73">
@@ -23341,7 +23341,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>13497860.72156341</v>
+        <v>153318143.2776757</v>
       </c>
     </row>
     <row r="74">
@@ -23352,7 +23352,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>11207527.10470622</v>
+        <v>168675674.4053533</v>
       </c>
     </row>
     <row r="75">
@@ -23363,7 +23363,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>15440612.55072757</v>
+        <v>68450695.08733051</v>
       </c>
     </row>
     <row r="76">
@@ -23374,7 +23374,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>15620210.06021401</v>
+        <v>68351352.22578388</v>
       </c>
     </row>
     <row r="77">
@@ -23385,7 +23385,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>15893586.88551395</v>
+        <v>68200136.11937186</v>
       </c>
     </row>
     <row r="78">
@@ -23396,7 +23396,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>15911556.98701414</v>
+        <v>68190196.10789612</v>
       </c>
     </row>
     <row r="79">
@@ -23407,7 +23407,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>15319467.61027232</v>
+        <v>68427248.43829936</v>
       </c>
     </row>
     <row r="80">
@@ -23418,7 +23418,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>14243718.05116007</v>
+        <v>69194714.34607965</v>
       </c>
     </row>
     <row r="81">
@@ -23429,7 +23429,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>11275000.89769531</v>
+        <v>167740800.5420159</v>
       </c>
     </row>
     <row r="82">
@@ -23440,7 +23440,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>11124494.19232186</v>
+        <v>154481804.7374096</v>
       </c>
     </row>
     <row r="83">
@@ -23451,7 +23451,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>12152981.52540478</v>
+        <v>152500103.9272394</v>
       </c>
     </row>
     <row r="84">
@@ -23462,7 +23462,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>12581292.31448059</v>
+        <v>68599802.95749058</v>
       </c>
     </row>
     <row r="85">
@@ -23473,7 +23473,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>15122915.3402404</v>
+        <v>68626426.64444079</v>
       </c>
     </row>
     <row r="86">
@@ -23484,7 +23484,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>15876296.16381384</v>
+        <v>68209700.33758852</v>
       </c>
     </row>
     <row r="87">
@@ -23495,7 +23495,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>14176555.26816908</v>
+        <v>155945587.8913524</v>
       </c>
     </row>
     <row r="88">
@@ -23506,7 +23506,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>9261435.489619618</v>
+        <v>160827496.1900521</v>
       </c>
     </row>
     <row r="89">
@@ -23517,7 +23517,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>7442771.263907343</v>
+        <v>172920535.6392345</v>
       </c>
     </row>
     <row r="90">
@@ -23528,7 +23528,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>10565127.57689347</v>
+        <v>162474881.7126663</v>
       </c>
     </row>
     <row r="91">
@@ -23539,7 +23539,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>15455227.81602237</v>
+        <v>68442610.77546673</v>
       </c>
     </row>
     <row r="92">
@@ -23550,7 +23550,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>13984897.69078986</v>
+        <v>155947773.8611678</v>
       </c>
     </row>
     <row r="93">
@@ -23561,7 +23561,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>11186207.21294427</v>
+        <v>154385716.815189</v>
       </c>
     </row>
     <row r="94">
@@ -23572,7 +23572,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>4617907.41124785</v>
+        <v>221779480.1235125</v>
       </c>
     </row>
   </sheetData>
@@ -23641,7 +23641,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>131058494.3254194</v>
       </c>
     </row>
     <row r="5">
@@ -23652,7 +23652,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>2413345.550477924</v>
       </c>
     </row>
     <row r="6">
@@ -23663,7 +23663,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>6389916.638403693</v>
       </c>
     </row>
     <row r="7">
@@ -23674,7 +23674,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>3273207.137508361</v>
       </c>
     </row>
     <row r="8">
@@ -23685,7 +23685,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>13052971.64697553</v>
       </c>
     </row>
     <row r="9">
@@ -23696,7 +23696,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>62669439.50292609</v>
       </c>
     </row>
     <row r="10">
@@ -23707,7 +23707,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>14218976.95938518</v>
       </c>
     </row>
     <row r="11">
@@ -23718,7 +23718,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>81913757.21180981</v>
       </c>
     </row>
     <row r="12">
@@ -23729,7 +23729,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>56900892.07707654</v>
       </c>
     </row>
     <row r="13">
@@ -23740,7 +23740,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>89612946.97781889</v>
       </c>
     </row>
     <row r="14">
@@ -23751,7 +23751,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>46601495.82963394</v>
       </c>
     </row>
     <row r="15">
@@ -23762,7 +23762,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>25263280.87574057</v>
       </c>
     </row>
     <row r="16">
@@ -23773,7 +23773,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>3505311.677364837</v>
       </c>
     </row>
     <row r="17">
@@ -23784,7 +23784,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>12362585.78928441</v>
       </c>
     </row>
     <row r="18">
@@ -23806,7 +23806,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>20544679.79412371</v>
       </c>
     </row>
     <row r="20">
@@ -23817,7 +23817,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>9221516.200067287</v>
       </c>
     </row>
     <row r="21">
@@ -23861,7 +23861,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>27049719.69364135</v>
       </c>
     </row>
     <row r="25">
@@ -23872,7 +23872,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>2500785.589685444</v>
       </c>
     </row>
     <row r="26">
@@ -23894,7 +23894,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>24969675.44928377</v>
       </c>
     </row>
     <row r="28">
@@ -23905,7 +23905,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>17341146.965811</v>
       </c>
     </row>
     <row r="29">
@@ -23916,7 +23916,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>897516.1433767601</v>
       </c>
     </row>
     <row r="30">
@@ -23927,7 +23927,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>10875893.53077593</v>
       </c>
     </row>
     <row r="31">
@@ -23960,7 +23960,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>1604513.983641973</v>
       </c>
     </row>
     <row r="34">
@@ -23971,7 +23971,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>1514455.115702026</v>
       </c>
     </row>
     <row r="35">
@@ -23982,7 +23982,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>4512586.177768977</v>
       </c>
     </row>
     <row r="36">
@@ -24004,7 +24004,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>25711934.32592976</v>
       </c>
     </row>
     <row r="38">
@@ -24026,7 +24026,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>6592020.096219346</v>
       </c>
     </row>
     <row r="40">
@@ -24037,7 +24037,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>18056634.81026576</v>
       </c>
     </row>
     <row r="41">
@@ -24048,7 +24048,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>7768088.890829278</v>
       </c>
     </row>
     <row r="42">
@@ -24059,7 +24059,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>10483150.99748746</v>
       </c>
     </row>
     <row r="43">
@@ -24081,7 +24081,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>28703882.62044868</v>
       </c>
     </row>
     <row r="45">
@@ -24103,7 +24103,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>11859969.41413697</v>
       </c>
     </row>
     <row r="47">
@@ -24125,7 +24125,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>3227111.003289381</v>
       </c>
     </row>
     <row r="49">
@@ -24158,7 +24158,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>15376211.59856968</v>
       </c>
     </row>
     <row r="52">
@@ -24169,7 +24169,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>2779710.842566059</v>
       </c>
     </row>
     <row r="53">
@@ -24213,7 +24213,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>45504329.5548698</v>
       </c>
     </row>
     <row r="57">
@@ -24224,7 +24224,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>109566193.6461836</v>
       </c>
     </row>
     <row r="58">
@@ -24268,7 +24268,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>11840968.5689971</v>
       </c>
     </row>
     <row r="62">
@@ -24312,7 +24312,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>13583999.53872117</v>
       </c>
     </row>
     <row r="66">
@@ -24334,7 +24334,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>24087477.17776694</v>
       </c>
     </row>
     <row r="68">
@@ -24345,7 +24345,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>19006758.92749269</v>
       </c>
     </row>
     <row r="69">
@@ -24356,7 +24356,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>18510975.02305213</v>
       </c>
     </row>
     <row r="70">
@@ -24367,7 +24367,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>27750750.75370498</v>
       </c>
     </row>
     <row r="71">
@@ -24378,7 +24378,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>86034346.43493161</v>
       </c>
     </row>
     <row r="72">
@@ -24389,7 +24389,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>35895280.64668925</v>
       </c>
     </row>
     <row r="73">
@@ -24400,7 +24400,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>1159385.304723936</v>
       </c>
     </row>
     <row r="74">
@@ -24411,7 +24411,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>19451777.02248556</v>
       </c>
     </row>
     <row r="75">
@@ -24488,7 +24488,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>18913531.76255902</v>
       </c>
     </row>
     <row r="82">
@@ -24499,7 +24499,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>3722322.668930554</v>
       </c>
     </row>
     <row r="83">
@@ -24510,7 +24510,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>717115.7294173833</v>
       </c>
     </row>
     <row r="84">
@@ -24554,7 +24554,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>3752662.345021758</v>
       </c>
     </row>
     <row r="88">
@@ -24565,7 +24565,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>11884662.58463526</v>
       </c>
     </row>
     <row r="89">
@@ -24576,7 +24576,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>25847757.70290992</v>
       </c>
     </row>
     <row r="90">
@@ -24587,7 +24587,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>13121289.47168456</v>
       </c>
     </row>
     <row r="91">
@@ -24609,7 +24609,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>4410608.288616428</v>
       </c>
     </row>
     <row r="93">
@@ -24620,7 +24620,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>3518111.486447579</v>
       </c>
     </row>
     <row r="94">
@@ -24631,7 +24631,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>77480174.59646749</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed typos in appending and exporting of SWP CVP delivery dataframes
</commit_message>
<xml_diff>
--- a/CaUWMET/output.xlsx
+++ b/CaUWMET/output.xlsx
@@ -38481,7 +38481,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>14555.867749</v>
+        <v>6162.460273999999</v>
       </c>
     </row>
     <row r="5">
@@ -38536,7 +38536,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>9809.657749</v>
+        <v>6449.970973</v>
       </c>
     </row>
     <row r="10">
@@ -38558,7 +38558,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>9809.657749</v>
+        <v>5602.2462</v>
       </c>
     </row>
     <row r="12">
@@ -38569,7 +38569,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>12612.657749</v>
+        <v>8664.420512000001</v>
       </c>
     </row>
     <row r="13">
@@ -38580,7 +38580,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>14555.867749</v>
+        <v>9170.807624999999</v>
       </c>
     </row>
     <row r="14">
@@ -38591,7 +38591,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>9809.657749</v>
+        <v>7411.444726</v>
       </c>
     </row>
     <row r="15">
@@ -38602,7 +38602,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>12612.657749</v>
+        <v>11300.97281</v>
       </c>
     </row>
     <row r="16">
@@ -38646,7 +38646,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>14555.867749</v>
+        <v>13889.06056</v>
       </c>
     </row>
     <row r="20">
@@ -38701,7 +38701,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>14555.867749</v>
+        <v>13026.70683</v>
       </c>
     </row>
     <row r="25">
@@ -38734,7 +38734,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>14555.867749</v>
+        <v>13281.15969</v>
       </c>
     </row>
     <row r="28">
@@ -38844,7 +38844,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>14555.867749</v>
+        <v>13188.30152</v>
       </c>
     </row>
     <row r="38">
@@ -38921,7 +38921,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>14555.867749</v>
+        <v>12836.42959</v>
       </c>
     </row>
     <row r="45">
@@ -39053,7 +39053,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>14555.867749</v>
+        <v>11335.50479</v>
       </c>
     </row>
     <row r="57">
@@ -39064,7 +39064,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>9809.657749</v>
+        <v>4641.139957</v>
       </c>
     </row>
     <row r="58">
@@ -39174,7 +39174,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>14555.867749</v>
+        <v>13394.67621</v>
       </c>
     </row>
     <row r="68">
@@ -39207,7 +39207,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>9809.657749</v>
+        <v>9098.65857</v>
       </c>
     </row>
     <row r="71">
@@ -39218,7 +39218,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>9809.657749</v>
+        <v>5450.100503</v>
       </c>
     </row>
     <row r="72">
@@ -39229,7 +39229,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>9809.657749</v>
+        <v>8265.179714</v>
       </c>
     </row>
     <row r="73">
@@ -39251,7 +39251,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>14555.867749</v>
+        <v>14055.63512</v>
       </c>
     </row>
     <row r="75">
@@ -39328,7 +39328,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>14555.867749</v>
+        <v>14140.41289</v>
       </c>
     </row>
     <row r="82">
@@ -39416,7 +39416,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>9809.657749</v>
+        <v>9325.389633000001</v>
       </c>
     </row>
     <row r="90">
@@ -39471,7 +39471,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>9809.657749</v>
+        <v>5776.075931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>